<commit_message>
more structur in osc listener
</commit_message>
<xml_diff>
--- a/00_doc/Launch Control.xlsx
+++ b/00_doc/Launch Control.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2140" yWindow="2280" windowWidth="26660" windowHeight="10900"/>
+    <workbookView xWindow="2140" yWindow="660" windowWidth="26660" windowHeight="14020"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
@@ -726,7 +726,7 @@
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14:J14"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>